<commit_message>
contains fixes for some results
</commit_message>
<xml_diff>
--- a/Result/size_10_1000_07.xlsx
+++ b/Result/size_10_1000_07.xlsx
@@ -4389,21 +4389,50 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1665280"/>
-        <c:axId val="1667072"/>
+        <c:axId val="155001216"/>
+        <c:axId val="155002752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1665280"/>
+        <c:axId val="155001216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>#nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1667072"/>
+        <c:txPr>
+          <a:bodyPr rot="5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="155002752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4411,18 +4440,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1667072"/>
+        <c:axId val="155002752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1665280"/>
+        <c:crossAx val="155001216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4449,13 +4497,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>115500</xdr:colOff>
+      <xdr:colOff>67875</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>173325</xdr:rowOff>
     </xdr:to>

</xml_diff>